<commit_message>
- added new models
</commit_message>
<xml_diff>
--- a/Apontamento.xlsx
+++ b/Apontamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projectgreen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20485EFD-5291-4CBF-94CE-EBC0EE0776B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95782D3B-9ED3-476C-A46D-45944051C9E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1084,6 +1084,30 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="F13:L13"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="F5:L5"/>
+    <mergeCell ref="F6:L6"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="F9:L9"/>
+    <mergeCell ref="F10:L10"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="F25:L25"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="F15:L15"/>
+    <mergeCell ref="F16:L16"/>
+    <mergeCell ref="F17:L17"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="F20:L20"/>
+    <mergeCell ref="F21:L21"/>
+    <mergeCell ref="F22:L22"/>
+    <mergeCell ref="F23:L23"/>
+    <mergeCell ref="F24:L24"/>
     <mergeCell ref="F32:L32"/>
     <mergeCell ref="F33:L33"/>
     <mergeCell ref="F34:L34"/>
@@ -1093,30 +1117,6 @@
     <mergeCell ref="F29:L29"/>
     <mergeCell ref="F30:L30"/>
     <mergeCell ref="F31:L31"/>
-    <mergeCell ref="F20:L20"/>
-    <mergeCell ref="F21:L21"/>
-    <mergeCell ref="F22:L22"/>
-    <mergeCell ref="F23:L23"/>
-    <mergeCell ref="F24:L24"/>
-    <mergeCell ref="F25:L25"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="F15:L15"/>
-    <mergeCell ref="F16:L16"/>
-    <mergeCell ref="F17:L17"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="F9:L9"/>
-    <mergeCell ref="F10:L10"/>
-    <mergeCell ref="F11:L11"/>
-    <mergeCell ref="F12:L12"/>
-    <mergeCell ref="F13:L13"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="F5:L5"/>
-    <mergeCell ref="F6:L6"/>
-    <mergeCell ref="F7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1128,7 +1128,7 @@
   <dimension ref="A2:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:L12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,6 +1139,7 @@
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1179,8 +1180,12 @@
       <c r="A4" s="1">
         <v>43709</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="4"/>
@@ -1191,12 +1196,11 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="3">
-        <f>(C4-B4) +(E4-D4)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="N4" s="3">
         <f>SUM(M4:M34)</f>
-        <v>0.16666666666666669</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1204,10 +1208,10 @@
         <v>43710</v>
       </c>
       <c r="B5" s="2">
-        <v>4.1666666666666664E-2</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C5" s="2">
-        <v>0.20833333333333334</v>
+        <v>0.625</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1220,7 +1224,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="3">
         <f>(C5-B5) +(E5-D5)</f>
-        <v>0.16666666666666669</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -1228,8 +1232,12 @@
       <c r="A6" s="1">
         <v>43711</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
@@ -1249,8 +1257,12 @@
       <c r="A7" s="1">
         <v>43712</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
@@ -1270,8 +1282,12 @@
       <c r="A8" s="1">
         <v>43713</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
@@ -1291,8 +1307,12 @@
       <c r="A9" s="1">
         <v>43714</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
@@ -1312,8 +1332,12 @@
       <c r="A10" s="1">
         <v>43715</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
@@ -1333,8 +1357,12 @@
       <c r="A11" s="1">
         <v>43716</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
@@ -1354,8 +1382,12 @@
       <c r="A12" s="1">
         <v>43717</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
@@ -1375,8 +1407,12 @@
       <c r="A13" s="1">
         <v>43718</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
@@ -1396,8 +1432,12 @@
       <c r="A14" s="1">
         <v>43719</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
@@ -1417,8 +1457,12 @@
       <c r="A15" s="1">
         <v>43720</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
@@ -1438,8 +1482,12 @@
       <c r="A16" s="1">
         <v>43721</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
@@ -1459,8 +1507,12 @@
       <c r="A17" s="1">
         <v>43722</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="4"/>
@@ -1480,8 +1532,12 @@
       <c r="A18" s="1">
         <v>43723</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="4"/>
@@ -1501,8 +1557,12 @@
       <c r="A19" s="1">
         <v>43724</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="4"/>
@@ -1522,8 +1582,12 @@
       <c r="A20" s="1">
         <v>43725</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="4"/>
@@ -1543,8 +1607,12 @@
       <c r="A21" s="1">
         <v>43726</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="4"/>
@@ -1564,8 +1632,12 @@
       <c r="A22" s="1">
         <v>43727</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="4"/>
@@ -1585,8 +1657,12 @@
       <c r="A23" s="1">
         <v>43728</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="4"/>
@@ -1606,8 +1682,12 @@
       <c r="A24" s="1">
         <v>43729</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="4"/>
@@ -1627,8 +1707,12 @@
       <c r="A25" s="1">
         <v>43730</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="4"/>
@@ -1648,8 +1732,12 @@
       <c r="A26" s="1">
         <v>43731</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="4"/>
@@ -1669,8 +1757,12 @@
       <c r="A27" s="1">
         <v>43732</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="4"/>
@@ -1690,8 +1782,12 @@
       <c r="A28" s="1">
         <v>43733</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="4"/>
@@ -1711,8 +1807,12 @@
       <c r="A29" s="1">
         <v>43734</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="4"/>
@@ -1732,8 +1832,12 @@
       <c r="A30" s="1">
         <v>43735</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="4"/>
@@ -1753,8 +1857,12 @@
       <c r="A31" s="1">
         <v>43736</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="4"/>
@@ -1774,8 +1882,12 @@
       <c r="A32" s="1">
         <v>43737</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="4"/>
@@ -1795,8 +1907,12 @@
       <c r="A33" s="1">
         <v>43738</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="4"/>
@@ -1830,12 +1946,21 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="F5:L5"/>
-    <mergeCell ref="F6:L6"/>
-    <mergeCell ref="F10:L10"/>
-    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="F34:L34"/>
+    <mergeCell ref="F29:L29"/>
+    <mergeCell ref="F28:L28"/>
+    <mergeCell ref="F23:L23"/>
+    <mergeCell ref="F22:L22"/>
+    <mergeCell ref="F26:L26"/>
+    <mergeCell ref="F25:L25"/>
+    <mergeCell ref="F24:L24"/>
+    <mergeCell ref="F21:L21"/>
+    <mergeCell ref="F20:L20"/>
+    <mergeCell ref="F33:L33"/>
+    <mergeCell ref="F32:L32"/>
+    <mergeCell ref="F31:L31"/>
+    <mergeCell ref="F30:L30"/>
+    <mergeCell ref="F27:L27"/>
     <mergeCell ref="F11:L11"/>
     <mergeCell ref="F9:L9"/>
     <mergeCell ref="F8:L8"/>
@@ -1848,21 +1973,12 @@
     <mergeCell ref="F12:L12"/>
     <mergeCell ref="F17:L17"/>
     <mergeCell ref="F16:L16"/>
-    <mergeCell ref="F21:L21"/>
-    <mergeCell ref="F20:L20"/>
-    <mergeCell ref="F33:L33"/>
-    <mergeCell ref="F32:L32"/>
-    <mergeCell ref="F31:L31"/>
-    <mergeCell ref="F30:L30"/>
-    <mergeCell ref="F27:L27"/>
-    <mergeCell ref="F34:L34"/>
-    <mergeCell ref="F29:L29"/>
-    <mergeCell ref="F28:L28"/>
-    <mergeCell ref="F23:L23"/>
-    <mergeCell ref="F22:L22"/>
-    <mergeCell ref="F26:L26"/>
-    <mergeCell ref="F25:L25"/>
-    <mergeCell ref="F24:L24"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="F5:L5"/>
+    <mergeCell ref="F6:L6"/>
+    <mergeCell ref="F10:L10"/>
+    <mergeCell ref="F4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>